<commit_message>
made notes notebook and analysis.md for github
</commit_message>
<xml_diff>
--- a/data/manual/not_confirmed_pregnant.xlsx
+++ b/data/manual/not_confirmed_pregnant.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R136"/>
+  <dimension ref="A1:S136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +526,11 @@
       <c r="R1" s="1" t="inlineStr">
         <is>
           <t>may_be_pregnant_rc_graf</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
         </is>
       </c>
     </row>
@@ -646,6 +651,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S2" t="n">
+        <v>2012</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -738,6 +746,9 @@
         </is>
       </c>
       <c r="R3" t="inlineStr"/>
+      <c r="S3" t="n">
+        <v>2016</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -824,6 +835,9 @@
         </is>
       </c>
       <c r="R4" t="inlineStr"/>
+      <c r="S4" t="n">
+        <v>2015</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -915,6 +929,9 @@
           <t>pregnan</t>
         </is>
       </c>
+      <c r="S5" t="n">
+        <v>2015</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1003,6 +1020,9 @@
         <is>
           <t>pregnan</t>
         </is>
+      </c>
+      <c r="S6" t="n">
+        <v>2015</v>
       </c>
     </row>
     <row r="7">
@@ -1102,6 +1122,9 @@
         </is>
       </c>
       <c r="R7" t="inlineStr"/>
+      <c r="S7" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1188,6 +1211,9 @@
         </is>
       </c>
       <c r="R8" t="inlineStr"/>
+      <c r="S8" t="n">
+        <v>2014</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1288,6 +1314,9 @@
         </is>
       </c>
       <c r="R9" t="inlineStr"/>
+      <c r="S9" t="n">
+        <v>2014</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1394,6 +1423,9 @@
           <t>pregnan</t>
         </is>
       </c>
+      <c r="S10" t="n">
+        <v>2013</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1488,6 +1520,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S11" t="n">
+        <v>2019</v>
       </c>
     </row>
     <row r="12">
@@ -1584,6 +1619,9 @@
         </is>
       </c>
       <c r="R12" t="inlineStr"/>
+      <c r="S12" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1737,6 +1775,9 @@
         </is>
       </c>
       <c r="R13" t="inlineStr"/>
+      <c r="S13" t="n">
+        <v>2021</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1964,6 +2005,9 @@
           <t>pregnan</t>
         </is>
       </c>
+      <c r="S14" t="n">
+        <v>2015</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -2060,6 +2104,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S15" t="n">
+        <v>2013</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -2153,6 +2200,9 @@
           <t>pregnan</t>
         </is>
       </c>
+      <c r="S16" t="n">
+        <v>2021</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2243,6 +2293,9 @@
         <is>
           <t>pregnan</t>
         </is>
+      </c>
+      <c r="S17" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="18">
@@ -2360,6 +2413,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S18" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="19">
@@ -2510,6 +2566,9 @@
         </is>
       </c>
       <c r="R19" t="inlineStr"/>
+      <c r="S19" t="n">
+        <v>2011</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -2598,6 +2657,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S20" t="n">
+        <v>2012</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -2685,6 +2747,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S21" t="n">
+        <v>2019</v>
       </c>
     </row>
     <row r="22">
@@ -2784,6 +2849,9 @@
         </is>
       </c>
       <c r="R22" t="inlineStr"/>
+      <c r="S22" t="n">
+        <v>2012</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2868,6 +2936,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S23" t="n">
+        <v>2014</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2950,6 +3021,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S24" t="n">
+        <v>2013</v>
       </c>
     </row>
     <row r="25">
@@ -3045,6 +3119,9 @@
           <t>active labor</t>
         </is>
       </c>
+      <c r="S25" t="n">
+        <v>2014</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -3141,6 +3218,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S26" t="n">
+        <v>2017</v>
       </c>
     </row>
     <row r="27">
@@ -3361,6 +3441,9 @@
         </is>
       </c>
       <c r="R27" t="inlineStr"/>
+      <c r="S27" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -3443,6 +3526,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S28" t="n">
+        <v>2019</v>
       </c>
     </row>
     <row r="29">
@@ -3622,6 +3708,9 @@
           <t>pregnan</t>
         </is>
       </c>
+      <c r="S29" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -3777,6 +3866,9 @@
           <t>pregnan</t>
         </is>
       </c>
+      <c r="S30" t="n">
+        <v>2020</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -3895,6 +3987,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S31" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -3980,6 +4075,9 @@
         </is>
       </c>
       <c r="R32" t="inlineStr"/>
+      <c r="S32" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -4093,6 +4191,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S33" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -4182,6 +4283,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S34" t="n">
+        <v>2014</v>
       </c>
     </row>
     <row r="35">
@@ -4280,6 +4384,9 @@
           <t>gestation</t>
         </is>
       </c>
+      <c r="S35" t="n">
+        <v>2020</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -4369,6 +4476,9 @@
         <is>
           <t>pregnan</t>
         </is>
+      </c>
+      <c r="S36" t="n">
+        <v>2011</v>
       </c>
     </row>
     <row r="37">
@@ -4467,6 +4577,9 @@
           <t>pregnan</t>
         </is>
       </c>
+      <c r="S37" t="n">
+        <v>2011</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -4557,6 +4670,9 @@
         <is>
           <t>pregnan</t>
         </is>
+      </c>
+      <c r="S38" t="n">
+        <v>2011</v>
       </c>
     </row>
     <row r="39">
@@ -4670,6 +4786,9 @@
           <t>pregnan</t>
         </is>
       </c>
+      <c r="S39" t="n">
+        <v>2013</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -4779,6 +4898,9 @@
           <t>pregnan</t>
         </is>
       </c>
+      <c r="S40" t="n">
+        <v>2013</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -4863,6 +4985,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S41" t="n">
+        <v>2013</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -4946,6 +5071,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S42" t="n">
+        <v>2013</v>
       </c>
     </row>
     <row r="43">
@@ -5049,6 +5177,9 @@
         <is>
           <t>pregnan</t>
         </is>
+      </c>
+      <c r="S43" t="n">
+        <v>2018</v>
       </c>
     </row>
     <row r="44">
@@ -5249,6 +5380,9 @@
           <t>pregnan</t>
         </is>
       </c>
+      <c r="S44" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -5369,6 +5503,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S45" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -5491,6 +5628,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S46" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -5590,6 +5730,9 @@
         </is>
       </c>
       <c r="R47" t="inlineStr"/>
+      <c r="S47" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -5680,6 +5823,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S48" t="n">
+        <v>2015</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -5767,6 +5913,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S49" t="n">
+        <v>2013</v>
       </c>
     </row>
     <row r="50">
@@ -5856,6 +6005,9 @@
           <t>gestation</t>
         </is>
       </c>
+      <c r="S50" t="n">
+        <v>2020</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -5946,6 +6098,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S51" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -6030,6 +6185,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S52" t="n">
+        <v>2020</v>
       </c>
     </row>
     <row r="53">
@@ -6118,6 +6276,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S53" t="n">
+        <v>2017</v>
       </c>
     </row>
     <row r="54">
@@ -6209,6 +6370,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S54" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -6294,6 +6458,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S55" t="n">
+        <v>2012</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -6382,6 +6549,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S56" t="n">
+        <v>2012</v>
       </c>
     </row>
     <row r="57">
@@ -6470,6 +6640,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S57" t="n">
+        <v>2012</v>
       </c>
     </row>
     <row r="58">
@@ -6563,6 +6736,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S58" t="n">
+        <v>2012</v>
       </c>
     </row>
     <row r="59">
@@ -6723,6 +6899,9 @@
         </is>
       </c>
       <c r="R59" t="inlineStr"/>
+      <c r="S59" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -6871,6 +7050,9 @@
         </is>
       </c>
       <c r="R60" t="inlineStr"/>
+      <c r="S60" t="n">
+        <v>2021</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -6954,6 +7136,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S61" t="n">
+        <v>2018</v>
       </c>
     </row>
     <row r="62">
@@ -7061,6 +7246,9 @@
         <is>
           <t>obstetr</t>
         </is>
+      </c>
+      <c r="S62" t="n">
+        <v>2022</v>
       </c>
     </row>
     <row r="63">
@@ -7196,6 +7384,9 @@
           <t>pregnan</t>
         </is>
       </c>
+      <c r="S63" t="n">
+        <v>2011</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -7279,6 +7470,9 @@
         </is>
       </c>
       <c r="R64" t="inlineStr"/>
+      <c r="S64" t="n">
+        <v>2016</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -7365,6 +7559,9 @@
           <t>obstetr</t>
         </is>
       </c>
+      <c r="S65" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -7461,6 +7658,9 @@
       </c>
       <c r="Q66" t="inlineStr"/>
       <c r="R66" t="inlineStr"/>
+      <c r="S66" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -7551,6 +7751,9 @@
       </c>
       <c r="Q67" t="inlineStr"/>
       <c r="R67" t="inlineStr"/>
+      <c r="S67" t="n">
+        <v>2014</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -7645,6 +7848,9 @@
       </c>
       <c r="Q68" t="inlineStr"/>
       <c r="R68" t="inlineStr"/>
+      <c r="S68" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -7746,6 +7952,9 @@
       </c>
       <c r="Q69" t="inlineStr"/>
       <c r="R69" t="inlineStr"/>
+      <c r="S69" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -7842,6 +8051,9 @@
       </c>
       <c r="Q70" t="inlineStr"/>
       <c r="R70" t="inlineStr"/>
+      <c r="S70" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -7933,6 +8145,9 @@
       </c>
       <c r="Q71" t="inlineStr"/>
       <c r="R71" t="inlineStr"/>
+      <c r="S71" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -8027,6 +8242,9 @@
       </c>
       <c r="Q72" t="inlineStr"/>
       <c r="R72" t="inlineStr"/>
+      <c r="S72" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -8117,6 +8335,9 @@
       </c>
       <c r="Q73" t="inlineStr"/>
       <c r="R73" t="inlineStr"/>
+      <c r="S73" t="n">
+        <v>2013</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -8210,6 +8431,9 @@
       </c>
       <c r="Q74" t="inlineStr"/>
       <c r="R74" t="inlineStr"/>
+      <c r="S74" t="n">
+        <v>2020</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -8424,6 +8648,9 @@
       </c>
       <c r="Q75" t="inlineStr"/>
       <c r="R75" t="inlineStr"/>
+      <c r="S75" t="n">
+        <v>2014</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -8517,6 +8744,9 @@
       </c>
       <c r="Q76" t="inlineStr"/>
       <c r="R76" t="inlineStr"/>
+      <c r="S76" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -8694,6 +8924,9 @@
       </c>
       <c r="Q77" t="inlineStr"/>
       <c r="R77" t="inlineStr"/>
+      <c r="S77" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -9095,6 +9328,9 @@
       </c>
       <c r="Q78" t="inlineStr"/>
       <c r="R78" t="inlineStr"/>
+      <c r="S78" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -9262,6 +9498,9 @@
       </c>
       <c r="Q79" t="inlineStr"/>
       <c r="R79" t="inlineStr"/>
+      <c r="S79" t="n">
+        <v>2020</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -9354,6 +9593,9 @@
       </c>
       <c r="Q80" t="inlineStr"/>
       <c r="R80" t="inlineStr"/>
+      <c r="S80" t="n">
+        <v>2011</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -9590,6 +9832,9 @@
       </c>
       <c r="Q81" t="inlineStr"/>
       <c r="R81" t="inlineStr"/>
+      <c r="S81" t="n">
+        <v>2011</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -9799,6 +10044,9 @@
       </c>
       <c r="Q82" t="inlineStr"/>
       <c r="R82" t="inlineStr"/>
+      <c r="S82" t="n">
+        <v>2015</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -9953,6 +10201,9 @@
       </c>
       <c r="Q83" t="inlineStr"/>
       <c r="R83" t="inlineStr"/>
+      <c r="S83" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -10075,6 +10326,9 @@
       </c>
       <c r="Q84" t="inlineStr"/>
       <c r="R84" t="inlineStr"/>
+      <c r="S84" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -10196,6 +10450,9 @@
       </c>
       <c r="Q85" t="inlineStr"/>
       <c r="R85" t="inlineStr"/>
+      <c r="S85" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -10299,6 +10556,9 @@
       </c>
       <c r="Q86" t="inlineStr"/>
       <c r="R86" t="inlineStr"/>
+      <c r="S86" t="n">
+        <v>2012</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -10424,6 +10684,9 @@
       </c>
       <c r="Q87" t="inlineStr"/>
       <c r="R87" t="inlineStr"/>
+      <c r="S87" t="n">
+        <v>2022</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -10541,6 +10804,9 @@
       </c>
       <c r="Q88" t="inlineStr"/>
       <c r="R88" t="inlineStr"/>
+      <c r="S88" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -10633,6 +10899,9 @@
       </c>
       <c r="Q89" t="inlineStr"/>
       <c r="R89" t="inlineStr"/>
+      <c r="S89" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -10747,6 +11016,9 @@
       </c>
       <c r="Q90" t="inlineStr"/>
       <c r="R90" t="inlineStr"/>
+      <c r="S90" t="n">
+        <v>2022</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -10886,6 +11158,9 @@
       </c>
       <c r="Q91" t="inlineStr"/>
       <c r="R91" t="inlineStr"/>
+      <c r="S91" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -11031,6 +11306,9 @@
       </c>
       <c r="Q92" t="inlineStr"/>
       <c r="R92" t="inlineStr"/>
+      <c r="S92" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -11196,6 +11474,9 @@
       </c>
       <c r="Q93" t="inlineStr"/>
       <c r="R93" t="inlineStr"/>
+      <c r="S93" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -11358,6 +11639,9 @@
       </c>
       <c r="Q94" t="inlineStr"/>
       <c r="R94" t="inlineStr"/>
+      <c r="S94" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -11453,6 +11737,9 @@
       </c>
       <c r="Q95" t="inlineStr"/>
       <c r="R95" t="inlineStr"/>
+      <c r="S95" t="n">
+        <v>2015</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -11696,6 +11983,9 @@
       </c>
       <c r="Q96" t="inlineStr"/>
       <c r="R96" t="inlineStr"/>
+      <c r="S96" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -11812,6 +12102,9 @@
       </c>
       <c r="Q97" t="inlineStr"/>
       <c r="R97" t="inlineStr"/>
+      <c r="S97" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -11919,6 +12212,9 @@
       </c>
       <c r="Q98" t="inlineStr"/>
       <c r="R98" t="inlineStr"/>
+      <c r="S98" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -12051,6 +12347,9 @@
       </c>
       <c r="Q99" t="inlineStr"/>
       <c r="R99" t="inlineStr"/>
+      <c r="S99" t="n">
+        <v>2011</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -12159,6 +12458,9 @@
       </c>
       <c r="Q100" t="inlineStr"/>
       <c r="R100" t="inlineStr"/>
+      <c r="S100" t="n">
+        <v>2015</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -12245,6 +12547,9 @@
       </c>
       <c r="Q101" t="inlineStr"/>
       <c r="R101" t="inlineStr"/>
+      <c r="S101" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -12372,6 +12677,9 @@
       </c>
       <c r="Q102" t="inlineStr"/>
       <c r="R102" t="inlineStr"/>
+      <c r="S102" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -12696,6 +13004,9 @@
       </c>
       <c r="Q103" t="inlineStr"/>
       <c r="R103" t="inlineStr"/>
+      <c r="S103" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -12820,6 +13131,9 @@
       </c>
       <c r="Q104" t="inlineStr"/>
       <c r="R104" t="inlineStr"/>
+      <c r="S104" t="n">
+        <v>2021</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -12904,6 +13218,9 @@
       </c>
       <c r="Q105" t="inlineStr"/>
       <c r="R105" t="inlineStr"/>
+      <c r="S105" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -13062,6 +13379,9 @@
       </c>
       <c r="Q106" t="inlineStr"/>
       <c r="R106" t="inlineStr"/>
+      <c r="S106" t="n">
+        <v>2014</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -13162,6 +13482,9 @@
       </c>
       <c r="Q107" t="inlineStr"/>
       <c r="R107" t="inlineStr"/>
+      <c r="S107" t="n">
+        <v>2016</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -13254,6 +13577,9 @@
       </c>
       <c r="Q108" t="inlineStr"/>
       <c r="R108" t="inlineStr"/>
+      <c r="S108" t="n">
+        <v>2012</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -13367,6 +13693,9 @@
       </c>
       <c r="Q109" t="inlineStr"/>
       <c r="R109" t="inlineStr"/>
+      <c r="S109" t="n">
+        <v>2011</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -13478,6 +13807,9 @@
       </c>
       <c r="Q110" t="inlineStr"/>
       <c r="R110" t="inlineStr"/>
+      <c r="S110" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -13565,6 +13897,9 @@
       </c>
       <c r="Q111" t="inlineStr"/>
       <c r="R111" t="inlineStr"/>
+      <c r="S111" t="n">
+        <v>2014</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -13654,6 +13989,9 @@
       </c>
       <c r="Q112" t="inlineStr"/>
       <c r="R112" t="inlineStr"/>
+      <c r="S112" t="n">
+        <v>2014</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -13748,6 +14086,9 @@
       </c>
       <c r="Q113" t="inlineStr"/>
       <c r="R113" t="inlineStr"/>
+      <c r="S113" t="n">
+        <v>2021</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -13865,6 +14206,9 @@
       </c>
       <c r="Q114" t="inlineStr"/>
       <c r="R114" t="inlineStr"/>
+      <c r="S114" t="n">
+        <v>2013</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -13955,6 +14299,9 @@
       </c>
       <c r="Q115" t="inlineStr"/>
       <c r="R115" t="inlineStr"/>
+      <c r="S115" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -14054,6 +14401,9 @@
       </c>
       <c r="Q116" t="inlineStr"/>
       <c r="R116" t="inlineStr"/>
+      <c r="S116" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -14149,6 +14499,9 @@
       </c>
       <c r="Q117" t="inlineStr"/>
       <c r="R117" t="inlineStr"/>
+      <c r="S117" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -14295,6 +14648,9 @@
       </c>
       <c r="Q118" t="inlineStr"/>
       <c r="R118" t="inlineStr"/>
+      <c r="S118" t="n">
+        <v>2022</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -14433,6 +14789,9 @@
       </c>
       <c r="Q119" t="inlineStr"/>
       <c r="R119" t="inlineStr"/>
+      <c r="S119" t="n">
+        <v>2015</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -14530,6 +14889,9 @@
       </c>
       <c r="Q120" t="inlineStr"/>
       <c r="R120" t="inlineStr"/>
+      <c r="S120" t="n">
+        <v>2012</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -14635,6 +14997,9 @@
       </c>
       <c r="Q121" t="inlineStr"/>
       <c r="R121" t="inlineStr"/>
+      <c r="S121" t="n">
+        <v>2012</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -14733,6 +15098,9 @@
       </c>
       <c r="Q122" t="inlineStr"/>
       <c r="R122" t="inlineStr"/>
+      <c r="S122" t="n">
+        <v>2016</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -14825,6 +15193,9 @@
       </c>
       <c r="Q123" t="inlineStr"/>
       <c r="R123" t="inlineStr"/>
+      <c r="S123" t="n">
+        <v>2016</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -14910,6 +15281,9 @@
       </c>
       <c r="Q124" t="inlineStr"/>
       <c r="R124" t="inlineStr"/>
+      <c r="S124" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -14996,6 +15370,9 @@
       </c>
       <c r="Q125" t="inlineStr"/>
       <c r="R125" t="inlineStr"/>
+      <c r="S125" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -15120,6 +15497,9 @@
       </c>
       <c r="Q126" t="inlineStr"/>
       <c r="R126" t="inlineStr"/>
+      <c r="S126" t="n">
+        <v>2020</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -15377,6 +15757,9 @@
       </c>
       <c r="Q127" t="inlineStr"/>
       <c r="R127" t="inlineStr"/>
+      <c r="S127" t="n">
+        <v>2014</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -15492,6 +15875,9 @@
       </c>
       <c r="Q128" t="inlineStr"/>
       <c r="R128" t="inlineStr"/>
+      <c r="S128" t="n">
+        <v>2016</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -15606,6 +15992,9 @@
       </c>
       <c r="Q129" t="inlineStr"/>
       <c r="R129" t="inlineStr"/>
+      <c r="S129" t="n">
+        <v>2016</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -15815,6 +16204,9 @@
       </c>
       <c r="Q130" t="inlineStr"/>
       <c r="R130" t="inlineStr"/>
+      <c r="S130" t="n">
+        <v>2021</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -15920,6 +16312,9 @@
       </c>
       <c r="Q131" t="inlineStr"/>
       <c r="R131" t="inlineStr"/>
+      <c r="S131" t="n">
+        <v>2011</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -16015,6 +16410,9 @@
       </c>
       <c r="Q132" t="inlineStr"/>
       <c r="R132" t="inlineStr"/>
+      <c r="S132" t="n">
+        <v>2019</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -16267,6 +16665,9 @@
       </c>
       <c r="Q133" t="inlineStr"/>
       <c r="R133" t="inlineStr"/>
+      <c r="S133" t="n">
+        <v>2017</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -16378,6 +16779,9 @@
       </c>
       <c r="Q134" t="inlineStr"/>
       <c r="R134" t="inlineStr"/>
+      <c r="S134" t="n">
+        <v>2018</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -16460,6 +16864,9 @@
       </c>
       <c r="Q135" t="inlineStr"/>
       <c r="R135" t="inlineStr"/>
+      <c r="S135" t="n">
+        <v>2016</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -16550,6 +16957,9 @@
       </c>
       <c r="Q136" t="inlineStr"/>
       <c r="R136" t="inlineStr"/>
+      <c r="S136" t="n">
+        <v>2018</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>